<commit_message>
pull data for scouting from other local data
</commit_message>
<xml_diff>
--- a/data/DreamLeague24-25.xlsx
+++ b/data/DreamLeague24-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kelloggcompany-my.sharepoint.com/personal/bryn_coombe_kellogg_com/Documents/Desktop/Dream League/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/462a734c48854128/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="534" documentId="8_{137F18B5-F53C-4947-B1E5-9555A7165B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AB1E453-9153-4EA2-A2B0-3FE3C354D46A}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{15BFD271-21FA-406A-A2D8-5C7B7CE6A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA8F07A2-07A0-4DD5-BBF8-07BBE9473144}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId1"/>
@@ -2018,9 +2018,6 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2044,6 +2041,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IX404"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:O18"/>
+    <sheetView showGridLines="0" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3355,11 +3355,11 @@
       <c r="O4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="122"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="130"/>
     </row>
     <row r="5" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="82"/>
@@ -3560,11 +3560,11 @@
       </c>
       <c r="M9" s="25">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N9" s="76">
         <f>SUM(F116:F133)</f>
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O9" s="77">
         <f>SUM(F113:F115)</f>
@@ -3616,11 +3616,11 @@
         <f>SUM(F140:F142)</f>
         <v>32</v>
       </c>
-      <c r="R10" s="122"/>
-      <c r="S10" s="122"/>
-      <c r="T10" s="122"/>
-      <c r="U10" s="122"/>
-      <c r="V10" s="122"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="130"/>
+      <c r="T10" s="130"/>
+      <c r="U10" s="130"/>
+      <c r="V10" s="130"/>
     </row>
     <row r="11" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="82"/>
@@ -3750,21 +3750,21 @@
       </c>
       <c r="M13" s="25">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N13" s="76">
         <f>SUM(F224:F241)</f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O13" s="77">
         <f>SUM(F221:F223)</f>
         <v>48</v>
       </c>
-      <c r="R13" s="122"/>
-      <c r="S13" s="122"/>
-      <c r="T13" s="122"/>
-      <c r="U13" s="122"/>
-      <c r="V13" s="122"/>
+      <c r="R13" s="130"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="130"/>
+      <c r="U13" s="130"/>
+      <c r="V13" s="130"/>
     </row>
     <row r="14" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="82"/>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="M16" s="25">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N16" s="26">
         <f>SUM(F305:F322)</f>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="O16" s="27">
         <f>SUM(F302:F304)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3948,11 +3948,11 @@
         <f>SUM(F329:F331)</f>
         <v>41</v>
       </c>
-      <c r="R17" s="122"/>
-      <c r="S17" s="122"/>
-      <c r="T17" s="122"/>
-      <c r="U17" s="122"/>
-      <c r="V17" s="122"/>
+      <c r="R17" s="130"/>
+      <c r="S17" s="130"/>
+      <c r="T17" s="130"/>
+      <c r="U17" s="130"/>
+      <c r="V17" s="130"/>
     </row>
     <row r="18" spans="1:22" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="82"/>
@@ -4056,11 +4056,11 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="R20" s="122"/>
-      <c r="S20" s="122"/>
-      <c r="T20" s="122"/>
-      <c r="U20" s="122"/>
-      <c r="V20" s="122"/>
+      <c r="R20" s="130"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="130"/>
+      <c r="V20" s="130"/>
     </row>
     <row r="21" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="82"/>
@@ -4184,11 +4184,11 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="R24" s="122"/>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="122"/>
-      <c r="V24" s="122"/>
+      <c r="R24" s="130"/>
+      <c r="S24" s="130"/>
+      <c r="T24" s="130"/>
+      <c r="U24" s="130"/>
+      <c r="V24" s="130"/>
     </row>
     <row r="25" spans="1:22" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="82"/>
@@ -4278,11 +4278,11 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="R28" s="122"/>
-      <c r="S28" s="122"/>
-      <c r="T28" s="122"/>
-      <c r="U28" s="122"/>
-      <c r="V28" s="122"/>
+      <c r="R28" s="130"/>
+      <c r="S28" s="130"/>
+      <c r="T28" s="130"/>
+      <c r="U28" s="130"/>
+      <c r="V28" s="130"/>
     </row>
     <row r="29" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
@@ -4523,11 +4523,11 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="R38" s="122"/>
-      <c r="S38" s="122"/>
-      <c r="T38" s="122"/>
-      <c r="U38" s="122"/>
-      <c r="V38" s="122"/>
+      <c r="R38" s="130"/>
+      <c r="S38" s="130"/>
+      <c r="T38" s="130"/>
+      <c r="U38" s="130"/>
+      <c r="V38" s="130"/>
     </row>
     <row r="39" spans="1:22" ht="13.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="82"/>
@@ -6544,7 +6544,7 @@
         <v>6</v>
       </c>
       <c r="F117" s="30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G117" s="89"/>
       <c r="H117" s="97"/>
@@ -6687,7 +6687,7 @@
         <v>274</v>
       </c>
       <c r="F122" s="30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G122" s="90">
         <v>45645</v>
@@ -6865,7 +6865,7 @@
         <v>274</v>
       </c>
       <c r="F128" s="30">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G128" s="90">
         <v>45617</v>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="F134" s="38">
         <f>SUM(F116:F133)-SUM(F113:F115)</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G134" s="83"/>
       <c r="H134" s="95"/>
@@ -9687,7 +9687,7 @@
         <v>274</v>
       </c>
       <c r="F241" s="30">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G241" s="90">
         <v>45589</v>
@@ -9712,7 +9712,7 @@
       </c>
       <c r="F242" s="38">
         <f>SUM(F224:F241)-SUM(F221:F223)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G242" s="83"/>
       <c r="H242" s="95"/>
@@ -11068,19 +11068,19 @@
     </row>
     <row r="295" spans="1:15" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A295" s="82"/>
-      <c r="B295" s="129" t="s">
+      <c r="B295" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="C295" s="130" t="s">
+      <c r="C295" s="129" t="s">
         <v>323</v>
       </c>
-      <c r="D295" s="130" t="s">
+      <c r="D295" s="129" t="s">
         <v>295</v>
       </c>
-      <c r="E295" s="124" t="s">
+      <c r="E295" s="123" t="s">
         <v>274</v>
       </c>
-      <c r="F295" s="125">
+      <c r="F295" s="124">
         <v>8</v>
       </c>
       <c r="G295" s="90">
@@ -11097,14 +11097,14 @@
     </row>
     <row r="296" spans="1:15" ht="13.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A296" s="1"/>
-      <c r="B296" s="123"/>
-      <c r="C296" s="123"/>
-      <c r="D296" s="123"/>
-      <c r="E296" s="127">
+      <c r="B296" s="122"/>
+      <c r="C296" s="122"/>
+      <c r="D296" s="122"/>
+      <c r="E296" s="126">
         <f>SUM(E275:E295)</f>
         <v>97</v>
       </c>
-      <c r="F296" s="128">
+      <c r="F296" s="127">
         <f>SUM(F278:F295)-SUM(F275:F276)</f>
         <v>46</v>
       </c>
@@ -11123,8 +11123,8 @@
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
       <c r="D297" s="1"/>
-      <c r="E297" s="126"/>
-      <c r="F297" s="123"/>
+      <c r="E297" s="125"/>
+      <c r="F297" s="122"/>
       <c r="G297" s="78"/>
       <c r="H297" s="78"/>
       <c r="I297" s="78"/>
@@ -11259,7 +11259,7 @@
         <v>274</v>
       </c>
       <c r="F303" s="21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G303" s="90">
         <v>45680</v>
@@ -11837,7 +11837,7 @@
       </c>
       <c r="F323" s="38">
         <f>SUM(F305:F322)-SUM(F302:F304)</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G323" s="83"/>
       <c r="H323" s="95"/>
@@ -13314,7 +13314,7 @@
   <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B20"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13438,10 +13438,10 @@
         <v>209</v>
       </c>
       <c r="E7" s="25">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F7" s="26">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G7" s="27">
         <v>31</v>
@@ -13588,13 +13588,13 @@
         <v>88</v>
       </c>
       <c r="E13" s="25">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F13" s="26">
         <v>74</v>
       </c>
       <c r="G13" s="27">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H13" s="55"/>
       <c r="I13" s="44"/>
@@ -13613,10 +13613,10 @@
         <v>66</v>
       </c>
       <c r="E14" s="25">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="59">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G14" s="60">
         <v>48</v>

</xml_diff>